<commit_message>
added a bunch of comments to improve understanding
</commit_message>
<xml_diff>
--- a/history/9709_12_2024_MayJune_Mathematics_qp_with_less_answers.xlsx
+++ b/history/9709_12_2024_MayJune_Mathematics_qp_with_less_answers.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,14 +476,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1(a)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -497,37 +497,284 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Too smart a monkey to receive such a score</t>
+          <t>Strong algebraic manipulation and trigonometric skills; good use of calculus (differentiation and integration) including chain rule and definite integrals; sequences and series handled accurately; coordinate geometry and circle/tangent questions well executed; geometry/trigonometry area/perimeter problems correctly structured and evaluated; rate-of-change problem solved cleanly.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Too dumb a human to perform so poor</t>
+          <t>Occasional difficulty with inequalities and determining intervals for monotonicity (Q9(a)); composition and inverse-function problem (Q4(c)) was missed; some confusion in constructing the perpendicular bisector with correct points and gradient (Q10(b)); presentation and clarity of reasoning could be improved to aid marking, especially in transformation descriptions and multi-step geometry proofs.</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1(b)</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3(a)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3(b)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4(a)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>4(b)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4(c)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5(a)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5(b)(i)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5(b)(ii)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6(a)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6(b)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>7(a)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>7(b)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>8(a)(i)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>8(a)(ii)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>8(b)</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>9(a)</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>9(b)</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10(a)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10(b)</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>6</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>